<commit_message>
change the filters to fromgroup
</commit_message>
<xml_diff>
--- a/אקסל ERD.xlsx
+++ b/אקסל ERD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\מרים ילין\Desktop\מסלול\פרקטיקום\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA2F476-9DD3-4A3A-B21D-89933401E756}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8340E6A4-1D24-4AFA-88AA-5329955E9243}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8964" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <sheet name="משימות אחרי שיחה עם מיכל" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -709,9 +710,6 @@
     </r>
   </si>
   <si>
-    <t>7.פרומגרופ לכל הסינונים</t>
-  </si>
-  <si>
     <t>8. לעשות שירות עם הפונקציה שמחזירה יתרת מלאי.מנוצלת /לא מנוצלת ושולחים לה כפרמטר לשכה, שנה או סוג תעודה?</t>
   </si>
   <si>
@@ -757,7 +755,28 @@
       </rPr>
       <t xml:space="preserve">
 בשנים - מתייחסים לתאריך טיפול
-להוסיף לטבלה ראשונה סינון לפי סוג תעודה
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>להוסיף לטבלה ראשונה סינון לפי סוג תעודה</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="177"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -771,12 +790,26 @@
       <t>להוסיף כפתור + של הוספת מלאי ליד הטבלה השניה (נמצא בגליון של מסכים) שמוסיף תעודות לטבלת REF OFFICE INVENTORY</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.פרומגרופ לכל הסינונים</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -818,6 +851,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1147,6 +1186,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1233,9 +1275,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1546,15 +1585,15 @@
     </row>
     <row r="4" spans="2:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="56" t="s">
+      <c r="E5" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="58"/>
-      <c r="H5" s="56" t="s">
+      <c r="F5" s="59"/>
+      <c r="H5" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="57"/>
-      <c r="J5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="59"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E6" s="1" t="s">
@@ -1653,10 +1692,10 @@
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E12" s="56" t="s">
+      <c r="E12" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="F12" s="58"/>
+      <c r="F12" s="59"/>
       <c r="H12" s="9" t="s">
         <v>9</v>
       </c>
@@ -1685,10 +1724,10 @@
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E14" s="65" t="s">
+      <c r="E14" s="66" t="s">
         <v>110</v>
       </c>
-      <c r="F14" s="66"/>
+      <c r="F14" s="67"/>
       <c r="H14" s="9" t="s">
         <v>11</v>
       </c>
@@ -1700,8 +1739,8 @@
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E15" s="65"/>
-      <c r="F15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="67"/>
       <c r="H15" s="9" t="s">
         <v>12</v>
       </c>
@@ -1713,8 +1752,8 @@
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E16" s="65"/>
-      <c r="F16" s="66"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="67"/>
       <c r="H16" s="9" t="s">
         <v>13</v>
       </c>
@@ -1726,8 +1765,8 @@
       </c>
     </row>
     <row r="17" spans="2:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E17" s="67"/>
-      <c r="F17" s="68"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="69"/>
       <c r="H17" s="9" t="s">
         <v>14</v>
       </c>
@@ -1750,13 +1789,13 @@
       </c>
     </row>
     <row r="19" spans="2:15" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="56" t="s">
+      <c r="B19" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="58"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="59"/>
       <c r="H19" s="10" t="s">
         <v>28</v>
       </c>
@@ -1801,17 +1840,17 @@
       <c r="F22" s="2">
         <v>2</v>
       </c>
-      <c r="H22" s="62" t="s">
+      <c r="H22" s="63" t="s">
         <v>98</v>
       </c>
-      <c r="I22" s="63"/>
-      <c r="J22" s="64"/>
-      <c r="L22" s="53" t="s">
+      <c r="I22" s="64"/>
+      <c r="J22" s="65"/>
+      <c r="L22" s="54" t="s">
         <v>130</v>
       </c>
-      <c r="M22" s="54"/>
-      <c r="N22" s="54"/>
-      <c r="O22" s="55"/>
+      <c r="M22" s="55"/>
+      <c r="N22" s="55"/>
+      <c r="O22" s="56"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="36"/>
@@ -1884,12 +1923,12 @@
       <c r="O25" s="7"/>
     </row>
     <row r="26" spans="2:15" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="59" t="s">
+      <c r="C26" s="60" t="s">
         <v>119</v>
       </c>
-      <c r="D26" s="60"/>
-      <c r="E26" s="60"/>
-      <c r="F26" s="61"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="62"/>
       <c r="H26" s="9" t="s">
         <v>46</v>
       </c>
@@ -1970,11 +2009,11 @@
     </row>
     <row r="32" spans="2:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="4:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D33" s="56" t="s">
+      <c r="D33" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="E33" s="57"/>
-      <c r="F33" s="58"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="59"/>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D34" s="38" t="s">
@@ -2078,11 +2117,11 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
-      <c r="J5" s="72" t="s">
+      <c r="J5" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="K5" s="73"/>
-      <c r="L5" s="74"/>
+      <c r="K5" s="74"/>
+      <c r="L5" s="75"/>
       <c r="M5" s="7"/>
     </row>
     <row r="6" spans="5:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2093,9 +2132,9 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="75"/>
-      <c r="K6" s="76"/>
-      <c r="L6" s="77"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="77"/>
+      <c r="L6" s="78"/>
       <c r="M6" s="7"/>
     </row>
     <row r="7" spans="5:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
@@ -2104,9 +2143,9 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="76"/>
-      <c r="L7" s="77"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="77"/>
+      <c r="L7" s="78"/>
       <c r="M7" s="7"/>
     </row>
     <row r="8" spans="5:13" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2121,9 +2160,9 @@
         <v>3</v>
       </c>
       <c r="I8" s="6"/>
-      <c r="J8" s="78"/>
-      <c r="K8" s="79"/>
-      <c r="L8" s="80"/>
+      <c r="J8" s="79"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="81"/>
       <c r="M8" s="7"/>
     </row>
     <row r="9" spans="5:13" x14ac:dyDescent="0.25">
@@ -2266,42 +2305,42 @@
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E22" s="8"/>
-      <c r="F22" s="69" t="s">
+      <c r="F22" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="G22" s="69"/>
-      <c r="H22" s="69"/>
-      <c r="I22" s="69"/>
-      <c r="J22" s="69"/>
-      <c r="K22" s="69"/>
-      <c r="L22" s="81" t="s">
+      <c r="G22" s="70"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="70"/>
+      <c r="J22" s="70"/>
+      <c r="K22" s="70"/>
+      <c r="L22" s="82" t="s">
         <v>67</v>
       </c>
       <c r="M22" s="24"/>
     </row>
     <row r="23" spans="2:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E23" s="8"/>
-      <c r="F23" s="69" t="s">
+      <c r="F23" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="G23" s="69"/>
-      <c r="H23" s="69"/>
-      <c r="I23" s="69"/>
-      <c r="J23" s="69"/>
-      <c r="K23" s="69"/>
-      <c r="L23" s="71"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="70"/>
+      <c r="I23" s="70"/>
+      <c r="J23" s="70"/>
+      <c r="K23" s="70"/>
+      <c r="L23" s="72"/>
       <c r="M23" s="24"/>
     </row>
     <row r="24" spans="2:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E24" s="8"/>
-      <c r="F24" s="69" t="s">
+      <c r="F24" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="G24" s="69"/>
-      <c r="H24" s="69"/>
-      <c r="I24" s="69"/>
-      <c r="J24" s="69"/>
-      <c r="K24" s="69"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="70"/>
+      <c r="I24" s="70"/>
+      <c r="J24" s="70"/>
+      <c r="K24" s="70"/>
       <c r="L24" s="23"/>
       <c r="M24" s="24"/>
     </row>
@@ -2310,15 +2349,15 @@
         <v>79</v>
       </c>
       <c r="E25" s="8"/>
-      <c r="F25" s="69" t="s">
+      <c r="F25" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="69"/>
-      <c r="H25" s="69"/>
-      <c r="I25" s="69"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="69"/>
-      <c r="L25" s="70" t="s">
+      <c r="G25" s="70"/>
+      <c r="H25" s="70"/>
+      <c r="I25" s="70"/>
+      <c r="J25" s="70"/>
+      <c r="K25" s="70"/>
+      <c r="L25" s="71" t="s">
         <v>69</v>
       </c>
       <c r="M25" s="24"/>
@@ -2328,120 +2367,120 @@
         <v>87</v>
       </c>
       <c r="E26" s="8"/>
-      <c r="F26" s="69" t="s">
+      <c r="F26" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="G26" s="69"/>
-      <c r="H26" s="69"/>
-      <c r="I26" s="69"/>
-      <c r="J26" s="69"/>
-      <c r="K26" s="69"/>
-      <c r="L26" s="71"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="70"/>
+      <c r="I26" s="70"/>
+      <c r="J26" s="70"/>
+      <c r="K26" s="70"/>
+      <c r="L26" s="72"/>
       <c r="M26" s="24"/>
     </row>
     <row r="27" spans="2:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E27" s="8"/>
-      <c r="F27" s="69" t="s">
+      <c r="F27" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="G27" s="69"/>
-      <c r="H27" s="69"/>
-      <c r="I27" s="69"/>
-      <c r="J27" s="69"/>
-      <c r="K27" s="69"/>
+      <c r="G27" s="70"/>
+      <c r="H27" s="70"/>
+      <c r="I27" s="70"/>
+      <c r="J27" s="70"/>
+      <c r="K27" s="70"/>
       <c r="L27" s="23"/>
       <c r="M27" s="24"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E28" s="8"/>
-      <c r="F28" s="69" t="s">
+      <c r="F28" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="G28" s="69"/>
-      <c r="H28" s="69"/>
-      <c r="I28" s="69"/>
-      <c r="J28" s="69"/>
-      <c r="K28" s="69"/>
-      <c r="L28" s="81" t="s">
+      <c r="G28" s="70"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="70"/>
+      <c r="J28" s="70"/>
+      <c r="K28" s="70"/>
+      <c r="L28" s="82" t="s">
         <v>84</v>
       </c>
       <c r="M28" s="24"/>
     </row>
     <row r="29" spans="2:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E29" s="8"/>
-      <c r="F29" s="69" t="s">
+      <c r="F29" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="G29" s="69"/>
-      <c r="H29" s="69"/>
-      <c r="I29" s="69"/>
-      <c r="J29" s="69"/>
-      <c r="K29" s="69"/>
-      <c r="L29" s="71"/>
+      <c r="G29" s="70"/>
+      <c r="H29" s="70"/>
+      <c r="I29" s="70"/>
+      <c r="J29" s="70"/>
+      <c r="K29" s="70"/>
+      <c r="L29" s="72"/>
       <c r="M29" s="24"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E30" s="8"/>
-      <c r="F30" s="69" t="s">
+      <c r="F30" s="70" t="s">
         <v>63</v>
       </c>
-      <c r="G30" s="69"/>
-      <c r="H30" s="69"/>
-      <c r="I30" s="69"/>
-      <c r="J30" s="69"/>
-      <c r="K30" s="69"/>
+      <c r="G30" s="70"/>
+      <c r="H30" s="70"/>
+      <c r="I30" s="70"/>
+      <c r="J30" s="70"/>
+      <c r="K30" s="70"/>
       <c r="L30" s="23"/>
       <c r="M30" s="24"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E31" s="8"/>
-      <c r="F31" s="69" t="s">
+      <c r="F31" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="G31" s="69"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="69"/>
-      <c r="J31" s="69"/>
-      <c r="K31" s="69"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="70"/>
+      <c r="I31" s="70"/>
+      <c r="J31" s="70"/>
+      <c r="K31" s="70"/>
       <c r="L31" s="23"/>
       <c r="M31" s="24"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E32" s="8"/>
-      <c r="F32" s="69" t="s">
+      <c r="F32" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="G32" s="69"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="69"/>
-      <c r="J32" s="69"/>
-      <c r="K32" s="69"/>
+      <c r="G32" s="70"/>
+      <c r="H32" s="70"/>
+      <c r="I32" s="70"/>
+      <c r="J32" s="70"/>
+      <c r="K32" s="70"/>
       <c r="L32" s="23"/>
       <c r="M32" s="24"/>
     </row>
     <row r="33" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E33" s="8"/>
-      <c r="F33" s="69" t="s">
+      <c r="F33" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="G33" s="69"/>
-      <c r="H33" s="69"/>
-      <c r="I33" s="69"/>
-      <c r="J33" s="69"/>
-      <c r="K33" s="69"/>
+      <c r="G33" s="70"/>
+      <c r="H33" s="70"/>
+      <c r="I33" s="70"/>
+      <c r="J33" s="70"/>
+      <c r="K33" s="70"/>
       <c r="L33" s="23"/>
       <c r="M33" s="24"/>
     </row>
     <row r="34" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E34" s="8"/>
-      <c r="F34" s="69" t="s">
+      <c r="F34" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="G34" s="69"/>
-      <c r="H34" s="69"/>
-      <c r="I34" s="69"/>
-      <c r="J34" s="69"/>
-      <c r="K34" s="69"/>
+      <c r="G34" s="70"/>
+      <c r="H34" s="70"/>
+      <c r="I34" s="70"/>
+      <c r="J34" s="70"/>
+      <c r="K34" s="70"/>
       <c r="L34" s="23"/>
       <c r="M34" s="24"/>
     </row>
@@ -2883,8 +2922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB54406D-6C29-4AA8-92AC-F13DD8010EA8}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2927,8 +2966,8 @@
       <c r="A4" s="43">
         <v>3</v>
       </c>
-      <c r="B4" s="82" t="s">
-        <v>149</v>
+      <c r="B4" s="53" t="s">
+        <v>148</v>
       </c>
       <c r="C4" s="43" t="s">
         <v>122</v>
@@ -3032,12 +3071,12 @@
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="51" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B18" s="51" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>